<commit_message>
fix: reports fixed - fix getStudentDeadlineReport Error
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/report-templates.xlsx
+++ b/src/main/resources/templates/report-templates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HikiCricel\Desktop\ВУЗ\3 курс 1 сем\Крос платформы\crossPlatform\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92ADDEE2-B285-43C5-B176-7F323CD36EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15561A4D-4712-42E9-B0D1-17834180475B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36495" yWindow="1605" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -89,9 +89,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Subject</t>
   </si>
   <si>
@@ -111,6 +108,9 @@
   </si>
   <si>
     <t>${student.name}</t>
+  </si>
+  <si>
+    <t>Student Name</t>
   </si>
 </sst>
 </file>
@@ -456,7 +456,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -469,30 +469,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>